<commit_message>
feat(documentation): update excel with end of survey pages
</commit_message>
<xml_diff>
--- a/src/documentation/LunaticSourceToEdt.xlsx
+++ b/src/documentation/LunaticSourceToEdt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isnmg\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isnmg\Documents\CARNET_EDT\carnet-web\edt\src\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400CE6D3-D506-4749-824F-5F23019A69A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD14EA9-ADEF-42D4-AC1E-7E390BF74DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{832AC5ED-4C8D-47A2-A1B2-A499903D6E99}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="98">
   <si>
     <t>4.1</t>
   </si>
@@ -168,11 +168,6 @@
   </si>
   <si>
     <t>WITHSOMEONE[i] = true</t>
-  </si>
-  <si>
-    <t>"IDREFSEARCH",
-"IDREFCATEGORY",
-"NEWACTIVITYLABEL"</t>
   </si>
   <si>
     <t>"STARTTIME",
@@ -218,10 +213,6 @@
 boolean[]</t>
   </si>
   <si>
-    <t>IDREFSEARCH[i] ||
- (NEWACTIVITYLABEL[i] &amp;&amp; !IDREFCATEGORY)</t>
-  </si>
-  <si>
     <t>DayOfSurvey</t>
   </si>
   <si>
@@ -285,20 +276,88 @@
     <t>"WEEKLYPLANNER"</t>
   </si>
   <si>
-    <t>String (JSON)</t>
-  </si>
-  <si>
     <t>KindOfWeek</t>
   </si>
   <si>
-    <t>"WORKINGWEEK",
-"HOLIDAYWEEK",
-"OTHERWEEK"</t>
-  </si>
-  <si>
-    <t>boolean,
-boolean,
-boolean</t>
+    <t>"GREATESTACTIVITYDAY"</t>
+  </si>
+  <si>
+    <t>"WORSTACTIVITYDAY"</t>
+  </si>
+  <si>
+    <t>"KINDOFDAY"</t>
+  </si>
+  <si>
+    <t>"EXCEPTIONALDAY"</t>
+  </si>
+  <si>
+    <t>"TRAVELTIME"</t>
+  </si>
+  <si>
+    <t>"PHONETIME"</t>
+  </si>
+  <si>
+    <t>CheckboxBooleanEdt</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>TravelTime</t>
+  </si>
+  <si>
+    <t>PhoneTime</t>
+  </si>
+  <si>
+    <t>ExceptionalDay</t>
+  </si>
+  <si>
+    <t>KindOfDay</t>
+  </si>
+  <si>
+    <t>WorstActivityDay</t>
+  </si>
+  <si>
+    <t>GreatestActivityDay</t>
+  </si>
+  <si>
+    <t>ISCLOTURE = true</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>EditActivityInformation</t>
+  </si>
+  <si>
+    <t>Input, Datepicker</t>
+  </si>
+  <si>
+    <t>"FIRSTNAME","SURVEYDATE"</t>
+  </si>
+  <si>
+    <t>String, String</t>
+  </si>
+  <si>
+    <t>On edit survey information</t>
+  </si>
+  <si>
+    <t>EditGlobalInformation</t>
+  </si>
+  <si>
+    <t>"FIRSTNAME", "SURVEYDATE"</t>
+  </si>
+  <si>
+    <t>"WEEKTYPE"</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>"MAINACTIVITY"</t>
+  </si>
+  <si>
+    <t>If activity was found using Autocomplete research or if that activity have been added</t>
   </si>
 </sst>
 </file>
@@ -359,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,6 +436,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,7 +748,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,12 +756,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089511AB-1E7D-4088-A1A0-D0D8C9BAA10E}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,25 +777,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>42</v>
@@ -738,67 +803,74 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="C4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -806,7 +878,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -814,7 +886,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -822,7 +894,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -830,7 +902,7 @@
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -843,16 +915,16 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -864,11 +936,11 @@
         <v>34</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="2" t="s">
-        <v>44</v>
+      <c r="F8" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>39</v>
@@ -876,7 +948,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -900,7 +972,7 @@
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -913,10 +985,10 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>40</v>
@@ -924,7 +996,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -946,7 +1018,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
@@ -970,7 +1042,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -992,7 +1064,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>
@@ -1012,9 +1084,9 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -1033,12 +1105,12 @@
         <v>31</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -1062,7 +1134,7 @@
     </row>
     <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>11</v>
@@ -1075,10 +1147,10 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>43</v>
@@ -1086,125 +1158,313 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1">
         <v>5</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="C18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>10</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E23" s="7"/>
       <c r="F23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1">
         <v>3</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC526F085CD1CA48ADFF716B92765F89" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="77eca9b8874b2dde324af9d571b7bba9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4dd11980-1879-4198-90e3-e88efa253408" xmlns:ns4="2a065d71-7238-4613-96cf-7562d4949755" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2abb8ba59b8be50596207cf711f9f340" ns3:_="" ns4:_="">
     <xsd:import namespace="4dd11980-1879-4198-90e3-e88efa253408"/>
@@ -1405,22 +1665,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02816655-BBB8-4149-993C-FD6F2D837E6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="2a065d71-7238-4613-96cf-7562d4949755"/>
+    <ds:schemaRef ds:uri="4dd11980-1879-4198-90e3-e88efa253408"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDF3A360-AF07-462B-8B01-09DA74F01B58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3AFDFF1-CE89-4150-A6F3-8C40ACF518F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1437,29 +1707,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDF3A360-AF07-462B-8B01-09DA74F01B58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02816655-BBB8-4149-993C-FD6F2D837E6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="2a065d71-7238-4613-96cf-7562d4949755"/>
-    <ds:schemaRef ds:uri="4dd11980-1879-4198-90e3-e88efa253408"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>